<commit_message>
changed Cofigurations in setup excel
</commit_message>
<xml_diff>
--- a/DataBaseRequirements.xlsx
+++ b/DataBaseRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\CCUv2\projects\eali-code-generator\AutocoderInputs\Excelsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excel_Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEB705C-58A3-4C78-B6D5-AF358DA4EBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E876BA-099E-44EF-A665-BF2A33156C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11325" tabRatio="272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configurations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8199" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8200" uniqueCount="1724">
   <si>
     <t>#Name CCU2 (Database)</t>
   </si>
@@ -5310,12 +5310,21 @@
   <si>
     <t>activePowerRateLimiter_frequencyFrtDuration</t>
   </si>
+  <si>
+    <t>enabled!</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5433,8 +5442,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5522,6 +5538,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -6001,7 +6023,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="16" borderId="10"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="11" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
@@ -6320,35 +6342,28 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="12" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6358,6 +6373,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6377,9 +6393,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="12" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6391,6 +6413,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -6692,11 +6717,11 @@
   <dimension ref="A1:AB468"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O424" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F421" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A269" sqref="A269:XFD269"/>
       <selection pane="topRight" activeCell="A269" sqref="A269:XFD269"/>
       <selection pane="bottomLeft" activeCell="A269" sqref="A269:XFD269"/>
-      <selection pane="bottomRight" activeCell="U453" sqref="U453"/>
+      <selection pane="bottomRight" activeCell="J399" sqref="J399:J456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -6736,34 +6761,34 @@
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="136"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="147"/>
       <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="124"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="130"/>
+      <c r="X1" s="130"/>
+      <c r="Y1" s="130"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6775,16 +6800,16 @@
       <c r="L2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="139" t="s">
+      <c r="M2" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="133"/>
-      <c r="O2" s="142" t="s">
+      <c r="N2" s="135"/>
+      <c r="O2" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="144"/>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="139"/>
+      <c r="R2" s="140"/>
       <c r="S2" s="29" t="s">
         <v>10</v>
       </c>
@@ -6794,11 +6819,11 @@
       <c r="U2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="132" t="s">
+      <c r="V2" s="144" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="128"/>
-      <c r="X2" s="133"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="135"/>
     </row>
     <row r="3" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -6899,7 +6924,7 @@
       <c r="I5" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="140"/>
+      <c r="J5" s="136"/>
       <c r="K5" s="70"/>
       <c r="L5" s="80" t="s">
         <v>41</v>
@@ -6958,7 +6983,7 @@
       <c r="I6" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="140"/>
+      <c r="J6" s="136"/>
       <c r="K6" s="70"/>
       <c r="L6" s="80" t="s">
         <v>41</v>
@@ -6989,33 +7014,33 @@
       </c>
     </row>
     <row r="7" spans="1:28" s="63" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="131" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="122"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="123"/>
-      <c r="O7" s="123"/>
-      <c r="P7" s="123"/>
-      <c r="Q7" s="123"/>
-      <c r="R7" s="123"/>
-      <c r="S7" s="123"/>
-      <c r="T7" s="123"/>
-      <c r="U7" s="123"/>
-      <c r="V7" s="123"/>
-      <c r="W7" s="123"/>
-      <c r="X7" s="123"/>
-      <c r="Y7" s="123"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="130"/>
+      <c r="T7" s="130"/>
+      <c r="U7" s="130"/>
+      <c r="V7" s="130"/>
+      <c r="W7" s="130"/>
+      <c r="X7" s="130"/>
+      <c r="Y7" s="130"/>
       <c r="Z7" s="103"/>
       <c r="AA7" s="103"/>
       <c r="AB7" s="103"/>
@@ -7046,7 +7071,7 @@
       <c r="I8" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="141" t="s">
+      <c r="J8" s="137" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="81" t="s">
@@ -7092,7 +7117,7 @@
       <c r="I9" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="130"/>
+      <c r="J9" s="125"/>
       <c r="L9" s="81" t="s">
         <v>41</v>
       </c>
@@ -7135,7 +7160,7 @@
       <c r="I10" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="130"/>
+      <c r="J10" s="125"/>
       <c r="L10" s="81" t="s">
         <v>41</v>
       </c>
@@ -7185,7 +7210,7 @@
       <c r="I11" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="130"/>
+      <c r="J11" s="125"/>
       <c r="L11" s="81" t="s">
         <v>41</v>
       </c>
@@ -7222,7 +7247,7 @@
       <c r="I12" t="s">
         <v>70</v>
       </c>
-      <c r="J12" s="130"/>
+      <c r="J12" s="125"/>
       <c r="L12" s="81" t="s">
         <v>41</v>
       </c>
@@ -7262,7 +7287,7 @@
       <c r="I13" t="s">
         <v>74</v>
       </c>
-      <c r="J13" s="130"/>
+      <c r="J13" s="125"/>
       <c r="L13" s="81" t="s">
         <v>41</v>
       </c>
@@ -7316,7 +7341,7 @@
       <c r="I15" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="131" t="s">
+      <c r="J15" s="124" t="s">
         <v>78</v>
       </c>
       <c r="L15" s="81" t="s">
@@ -7356,7 +7381,7 @@
       <c r="I16" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="130"/>
+      <c r="J16" s="125"/>
       <c r="L16" s="81" t="s">
         <v>41</v>
       </c>
@@ -7394,7 +7419,7 @@
       <c r="I17" t="s">
         <v>84</v>
       </c>
-      <c r="J17" s="130"/>
+      <c r="J17" s="125"/>
       <c r="L17" s="81" t="s">
         <v>41</v>
       </c>
@@ -7433,7 +7458,7 @@
       <c r="I18" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="130"/>
+      <c r="J18" s="125"/>
       <c r="L18" s="81" t="s">
         <v>41</v>
       </c>
@@ -7542,7 +7567,7 @@
       <c r="I22" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="131" t="s">
+      <c r="J22" s="124" t="s">
         <v>78</v>
       </c>
       <c r="K22" s="70"/>
@@ -7587,7 +7612,7 @@
       <c r="I23" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="130"/>
+      <c r="J23" s="125"/>
       <c r="K23" s="70"/>
       <c r="L23" s="79" t="s">
         <v>93</v>
@@ -7630,7 +7655,7 @@
       <c r="I24" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="130"/>
+      <c r="J24" s="125"/>
       <c r="K24" s="70"/>
       <c r="L24" s="79" t="s">
         <v>93</v>
@@ -7651,33 +7676,33 @@
       <c r="X24" s="3"/>
     </row>
     <row r="25" spans="1:28" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="122" t="s">
+      <c r="A25" s="131" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="122"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="123"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="123"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="123"/>
-      <c r="L25" s="123"/>
-      <c r="M25" s="123"/>
-      <c r="N25" s="123"/>
-      <c r="O25" s="123"/>
-      <c r="P25" s="123"/>
-      <c r="Q25" s="123"/>
-      <c r="R25" s="123"/>
-      <c r="S25" s="123"/>
-      <c r="T25" s="123"/>
-      <c r="U25" s="123"/>
-      <c r="V25" s="123"/>
-      <c r="W25" s="123"/>
-      <c r="X25" s="123"/>
-      <c r="Y25" s="123"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+      <c r="K25" s="130"/>
+      <c r="L25" s="130"/>
+      <c r="M25" s="130"/>
+      <c r="N25" s="130"/>
+      <c r="O25" s="130"/>
+      <c r="P25" s="130"/>
+      <c r="Q25" s="130"/>
+      <c r="R25" s="130"/>
+      <c r="S25" s="130"/>
+      <c r="T25" s="130"/>
+      <c r="U25" s="130"/>
+      <c r="V25" s="130"/>
+      <c r="W25" s="130"/>
+      <c r="X25" s="130"/>
+      <c r="Y25" s="130"/>
       <c r="Z25" s="103"/>
       <c r="AA25" s="103"/>
       <c r="AB25" s="103"/>
@@ -7706,7 +7731,7 @@
       <c r="I26" t="s">
         <v>104</v>
       </c>
-      <c r="J26" s="131" t="s">
+      <c r="J26" s="124" t="s">
         <v>78</v>
       </c>
       <c r="L26" s="80" t="s">
@@ -7745,7 +7770,7 @@
       <c r="I27" t="s">
         <v>107</v>
       </c>
-      <c r="J27" s="130"/>
+      <c r="J27" s="125"/>
       <c r="L27" s="80" t="s">
         <v>41</v>
       </c>
@@ -7761,7 +7786,7 @@
         <v>108</v>
       </c>
       <c r="B28" s="106"/>
-      <c r="C28" s="137" t="s">
+      <c r="C28" s="132" t="s">
         <v>1424</v>
       </c>
       <c r="D28" s="56"/>
@@ -7780,7 +7805,7 @@
       <c r="I28" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="130"/>
+      <c r="J28" s="125"/>
       <c r="L28" s="80" t="s">
         <v>41</v>
       </c>
@@ -7796,7 +7821,7 @@
         <v>109</v>
       </c>
       <c r="B29" s="106"/>
-      <c r="C29" s="138"/>
+      <c r="C29" s="133"/>
       <c r="D29" s="56"/>
       <c r="E29" s="68" t="s">
         <v>48</v>
@@ -7813,7 +7838,7 @@
       <c r="I29" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="130"/>
+      <c r="J29" s="125"/>
       <c r="L29" s="80" t="s">
         <v>41</v>
       </c>
@@ -7829,7 +7854,7 @@
         <v>113</v>
       </c>
       <c r="B30" s="106"/>
-      <c r="C30" s="138"/>
+      <c r="C30" s="133"/>
       <c r="D30" s="56"/>
       <c r="E30" s="68" t="s">
         <v>48</v>
@@ -7846,7 +7871,7 @@
       <c r="I30" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="130"/>
+      <c r="J30" s="125"/>
       <c r="L30" s="80" t="s">
         <v>41</v>
       </c>
@@ -7862,7 +7887,7 @@
         <v>114</v>
       </c>
       <c r="B31" s="106"/>
-      <c r="C31" s="138"/>
+      <c r="C31" s="133"/>
       <c r="D31" s="56"/>
       <c r="E31" s="68" t="s">
         <v>48</v>
@@ -7879,7 +7904,7 @@
       <c r="I31" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="130"/>
+      <c r="J31" s="125"/>
       <c r="L31" s="80" t="s">
         <v>41</v>
       </c>
@@ -7895,7 +7920,7 @@
         <v>117</v>
       </c>
       <c r="B32" s="106"/>
-      <c r="C32" s="138"/>
+      <c r="C32" s="133"/>
       <c r="D32" s="56"/>
       <c r="E32" s="68" t="s">
         <v>48</v>
@@ -7912,7 +7937,7 @@
       <c r="I32" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="130"/>
+      <c r="J32" s="125"/>
       <c r="L32" s="80" t="s">
         <v>41</v>
       </c>
@@ -7928,7 +7953,7 @@
         <v>118</v>
       </c>
       <c r="B33" s="106"/>
-      <c r="C33" s="138"/>
+      <c r="C33" s="133"/>
       <c r="D33" s="56"/>
       <c r="E33" s="68" t="s">
         <v>48</v>
@@ -7945,7 +7970,7 @@
       <c r="I33" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="130"/>
+      <c r="J33" s="125"/>
       <c r="L33" s="80" t="s">
         <v>41</v>
       </c>
@@ -7961,7 +7986,7 @@
         <v>122</v>
       </c>
       <c r="B34" s="106"/>
-      <c r="C34" s="138"/>
+      <c r="C34" s="133"/>
       <c r="D34" s="56"/>
       <c r="E34" s="68" t="s">
         <v>48</v>
@@ -7978,7 +8003,7 @@
       <c r="I34" t="s">
         <v>35</v>
       </c>
-      <c r="J34" s="130"/>
+      <c r="J34" s="125"/>
       <c r="L34" s="80" t="s">
         <v>41</v>
       </c>
@@ -8013,7 +8038,7 @@
       <c r="I35" t="s">
         <v>35</v>
       </c>
-      <c r="J35" s="130"/>
+      <c r="J35" s="125"/>
       <c r="L35" s="80" t="s">
         <v>41</v>
       </c>
@@ -8048,7 +8073,7 @@
       <c r="I36" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="130"/>
+      <c r="J36" s="125"/>
       <c r="L36" s="80" t="s">
         <v>41</v>
       </c>
@@ -8144,7 +8169,7 @@
       <c r="I39" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="J39" s="130"/>
+      <c r="J39" s="125"/>
       <c r="L39" s="81" t="s">
         <v>41</v>
       </c>
@@ -8178,7 +8203,7 @@
       <c r="I40" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="J40" s="130"/>
+      <c r="J40" s="125"/>
       <c r="L40" s="81" t="s">
         <v>41</v>
       </c>
@@ -8215,7 +8240,7 @@
       <c r="I41" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="J41" s="130"/>
+      <c r="J41" s="125"/>
       <c r="L41" s="81" t="s">
         <v>41</v>
       </c>
@@ -8249,7 +8274,7 @@
       <c r="I42" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="J42" s="130"/>
+      <c r="J42" s="125"/>
       <c r="L42" s="81" t="s">
         <v>41</v>
       </c>
@@ -8286,7 +8311,7 @@
       <c r="I43" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="J43" s="130"/>
+      <c r="J43" s="125"/>
       <c r="L43" s="81" t="s">
         <v>41</v>
       </c>
@@ -8320,7 +8345,7 @@
       <c r="I44" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="J44" s="130"/>
+      <c r="J44" s="125"/>
       <c r="L44" s="81" t="s">
         <v>41</v>
       </c>
@@ -8357,7 +8382,7 @@
       <c r="I45" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="J45" s="130"/>
+      <c r="J45" s="125"/>
       <c r="L45" s="81" t="s">
         <v>41</v>
       </c>
@@ -8392,7 +8417,7 @@
       <c r="I46" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="J46" s="130"/>
+      <c r="J46" s="125"/>
       <c r="L46" s="81" t="s">
         <v>41</v>
       </c>
@@ -8427,7 +8452,7 @@
       <c r="I47" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="J47" s="130"/>
+      <c r="J47" s="125"/>
       <c r="L47" s="81" t="s">
         <v>41</v>
       </c>
@@ -8462,7 +8487,7 @@
       <c r="I48" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="J48" s="130"/>
+      <c r="J48" s="125"/>
       <c r="L48" s="81" t="s">
         <v>41</v>
       </c>
@@ -8497,7 +8522,7 @@
       <c r="I49" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="J49" s="130"/>
+      <c r="J49" s="125"/>
       <c r="L49" s="81" t="s">
         <v>41</v>
       </c>
@@ -8534,7 +8559,7 @@
       <c r="I50" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J50" s="130"/>
+      <c r="J50" s="125"/>
       <c r="L50" s="81" t="s">
         <v>41</v>
       </c>
@@ -8578,7 +8603,7 @@
       <c r="I51" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="J51" s="130"/>
+      <c r="J51" s="125"/>
       <c r="L51" s="81" t="s">
         <v>41</v>
       </c>
@@ -8625,7 +8650,7 @@
       <c r="I52" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J52" s="130"/>
+      <c r="J52" s="125"/>
       <c r="L52" s="81" t="s">
         <v>41</v>
       </c>
@@ -8669,7 +8694,7 @@
       <c r="I53" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="J53" s="130"/>
+      <c r="J53" s="125"/>
       <c r="L53" s="81" t="s">
         <v>41</v>
       </c>
@@ -8716,7 +8741,7 @@
       <c r="I54" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J54" s="130"/>
+      <c r="J54" s="125"/>
       <c r="L54" s="81" t="s">
         <v>41</v>
       </c>
@@ -8760,7 +8785,7 @@
       <c r="I55" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="J55" s="130"/>
+      <c r="J55" s="125"/>
       <c r="L55" s="81" t="s">
         <v>41</v>
       </c>
@@ -8807,7 +8832,7 @@
       <c r="I56" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J56" s="130"/>
+      <c r="J56" s="125"/>
       <c r="L56" s="81" t="s">
         <v>41</v>
       </c>
@@ -8852,7 +8877,7 @@
       <c r="I57" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="J57" s="130"/>
+      <c r="J57" s="125"/>
       <c r="L57" s="81" t="s">
         <v>41</v>
       </c>
@@ -8899,7 +8924,7 @@
       <c r="I58" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J58" s="130"/>
+      <c r="J58" s="125"/>
       <c r="L58" s="81" t="s">
         <v>41</v>
       </c>
@@ -8946,7 +8971,7 @@
       <c r="I59" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J59" s="130"/>
+      <c r="J59" s="125"/>
       <c r="L59" s="81" t="s">
         <v>41</v>
       </c>
@@ -8993,7 +9018,7 @@
       <c r="I60" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J60" s="130"/>
+      <c r="J60" s="125"/>
       <c r="L60" s="81" t="s">
         <v>41</v>
       </c>
@@ -9040,7 +9065,7 @@
       <c r="I61" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J61" s="130"/>
+      <c r="J61" s="125"/>
       <c r="L61" s="81" t="s">
         <v>41</v>
       </c>
@@ -12113,33 +12138,33 @@
       <c r="X133" s="107"/>
     </row>
     <row r="134" spans="1:28" s="63" customFormat="1" ht="16.149999999999999" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="122" t="s">
+      <c r="A134" s="131" t="s">
         <v>254</v>
       </c>
-      <c r="B134" s="122"/>
-      <c r="C134" s="123"/>
-      <c r="D134" s="123"/>
-      <c r="E134" s="123"/>
-      <c r="F134" s="123"/>
-      <c r="G134" s="123"/>
-      <c r="H134" s="123"/>
-      <c r="I134" s="123"/>
-      <c r="J134" s="123"/>
-      <c r="K134" s="123"/>
-      <c r="L134" s="123"/>
-      <c r="M134" s="123"/>
-      <c r="N134" s="123"/>
-      <c r="O134" s="123"/>
-      <c r="P134" s="123"/>
-      <c r="Q134" s="123"/>
-      <c r="R134" s="123"/>
-      <c r="S134" s="123"/>
-      <c r="T134" s="123"/>
-      <c r="U134" s="123"/>
-      <c r="V134" s="123"/>
-      <c r="W134" s="123"/>
-      <c r="X134" s="123"/>
-      <c r="Y134" s="123"/>
+      <c r="B134" s="131"/>
+      <c r="C134" s="130"/>
+      <c r="D134" s="130"/>
+      <c r="E134" s="130"/>
+      <c r="F134" s="130"/>
+      <c r="G134" s="130"/>
+      <c r="H134" s="130"/>
+      <c r="I134" s="130"/>
+      <c r="J134" s="130"/>
+      <c r="K134" s="130"/>
+      <c r="L134" s="130"/>
+      <c r="M134" s="130"/>
+      <c r="N134" s="130"/>
+      <c r="O134" s="130"/>
+      <c r="P134" s="130"/>
+      <c r="Q134" s="130"/>
+      <c r="R134" s="130"/>
+      <c r="S134" s="130"/>
+      <c r="T134" s="130"/>
+      <c r="U134" s="130"/>
+      <c r="V134" s="130"/>
+      <c r="W134" s="130"/>
+      <c r="X134" s="130"/>
+      <c r="Y134" s="130"/>
       <c r="Z134" s="103"/>
       <c r="AA134" s="103"/>
       <c r="AB134" s="103"/>
@@ -14247,7 +14272,7 @@
       <c r="I184" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J184" s="131" t="s">
+      <c r="J184" s="124" t="s">
         <v>36</v>
       </c>
       <c r="L184" s="81" t="s">
@@ -14285,7 +14310,7 @@
       <c r="I185" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J185" s="130"/>
+      <c r="J185" s="125"/>
       <c r="L185" s="81" t="s">
         <v>41</v>
       </c>
@@ -14321,7 +14346,7 @@
       <c r="I186" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J186" s="130"/>
+      <c r="J186" s="125"/>
       <c r="L186" s="81" t="s">
         <v>41</v>
       </c>
@@ -14354,7 +14379,7 @@
       <c r="I187" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J187" s="130"/>
+      <c r="J187" s="125"/>
       <c r="L187" s="81" t="s">
         <v>41</v>
       </c>
@@ -14387,7 +14412,7 @@
       <c r="I188" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J188" s="130"/>
+      <c r="J188" s="125"/>
       <c r="L188" s="81" t="s">
         <v>41</v>
       </c>
@@ -14417,7 +14442,7 @@
       <c r="I189" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J189" s="130"/>
+      <c r="J189" s="125"/>
       <c r="L189" s="81" t="s">
         <v>41</v>
       </c>
@@ -14453,7 +14478,7 @@
       <c r="I190" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J190" s="130"/>
+      <c r="J190" s="125"/>
       <c r="L190" s="81"/>
       <c r="M190" s="94" t="s">
         <v>37</v>
@@ -14487,7 +14512,7 @@
       <c r="I191" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J191" s="130"/>
+      <c r="J191" s="125"/>
       <c r="L191" s="81"/>
       <c r="M191" s="94" t="s">
         <v>37</v>
@@ -14521,7 +14546,7 @@
       <c r="I192" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J192" s="130"/>
+      <c r="J192" s="125"/>
       <c r="L192" s="81"/>
       <c r="M192" s="94" t="s">
         <v>37</v>
@@ -14555,7 +14580,7 @@
       <c r="I193" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J193" s="130"/>
+      <c r="J193" s="125"/>
       <c r="L193" s="81"/>
       <c r="M193" s="94" t="s">
         <v>37</v>
@@ -14589,7 +14614,7 @@
       <c r="I194" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J194" s="130"/>
+      <c r="J194" s="125"/>
       <c r="L194" s="81"/>
       <c r="M194" s="94" t="s">
         <v>37</v>
@@ -14624,7 +14649,7 @@
       <c r="I195" t="s">
         <v>329</v>
       </c>
-      <c r="J195" s="130"/>
+      <c r="J195" s="125"/>
       <c r="L195" s="81" t="s">
         <v>41</v>
       </c>
@@ -14657,7 +14682,7 @@
       <c r="I196" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J196" s="130"/>
+      <c r="J196" s="125"/>
       <c r="L196" s="81" t="s">
         <v>41</v>
       </c>
@@ -14687,7 +14712,7 @@
       <c r="I197" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J197" s="130"/>
+      <c r="J197" s="125"/>
       <c r="L197" s="81" t="s">
         <v>41</v>
       </c>
@@ -14717,7 +14742,7 @@
       <c r="I198" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J198" s="130"/>
+      <c r="J198" s="125"/>
       <c r="L198" s="81" t="s">
         <v>41</v>
       </c>
@@ -14747,7 +14772,7 @@
       <c r="I199" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J199" s="130"/>
+      <c r="J199" s="125"/>
       <c r="L199" s="81"/>
       <c r="M199" s="94" t="s">
         <v>37</v>
@@ -14775,7 +14800,7 @@
       <c r="I200" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J200" s="130"/>
+      <c r="J200" s="125"/>
       <c r="L200" s="81"/>
       <c r="M200" s="94" t="s">
         <v>37</v>
@@ -14803,7 +14828,7 @@
       <c r="I201" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J201" s="130"/>
+      <c r="J201" s="125"/>
       <c r="L201" s="81"/>
       <c r="M201" s="94" t="s">
         <v>37</v>
@@ -14831,7 +14856,7 @@
       <c r="I202" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J202" s="130"/>
+      <c r="J202" s="125"/>
       <c r="L202" s="81"/>
       <c r="M202" s="94" t="s">
         <v>37</v>
@@ -14859,7 +14884,7 @@
       <c r="I203" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J203" s="130"/>
+      <c r="J203" s="125"/>
       <c r="L203" s="81"/>
       <c r="M203" s="94" t="s">
         <v>37</v>
@@ -14887,7 +14912,7 @@
       <c r="I204" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J204" s="130"/>
+      <c r="J204" s="125"/>
       <c r="L204" s="81"/>
       <c r="M204" s="94" t="s">
         <v>37</v>
@@ -14915,7 +14940,7 @@
       <c r="I205" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J205" s="130"/>
+      <c r="J205" s="125"/>
       <c r="L205" s="81"/>
       <c r="M205" s="94" t="s">
         <v>37</v>
@@ -14943,7 +14968,7 @@
       <c r="I206" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J206" s="130"/>
+      <c r="J206" s="125"/>
       <c r="L206" s="81"/>
       <c r="M206" s="94" t="s">
         <v>37</v>
@@ -14971,7 +14996,7 @@
       <c r="I207" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J207" s="130"/>
+      <c r="J207" s="125"/>
       <c r="L207" s="81"/>
       <c r="M207" s="94" t="s">
         <v>37</v>
@@ -15002,7 +15027,7 @@
       <c r="I208" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J208" s="130"/>
+      <c r="J208" s="125"/>
       <c r="L208" s="81" t="s">
         <v>41</v>
       </c>
@@ -15035,7 +15060,7 @@
       <c r="I209" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J209" s="130"/>
+      <c r="J209" s="125"/>
       <c r="L209" s="81"/>
       <c r="M209" s="94" t="s">
         <v>37</v>
@@ -15070,7 +15095,7 @@
       <c r="I210" t="s">
         <v>35</v>
       </c>
-      <c r="J210" s="130"/>
+      <c r="J210" s="125"/>
       <c r="L210" s="81" t="s">
         <v>41</v>
       </c>
@@ -15101,7 +15126,7 @@
       <c r="I211" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J211" s="130"/>
+      <c r="J211" s="125"/>
       <c r="L211" s="81"/>
       <c r="M211" s="94"/>
       <c r="U211" s="17" t="s">
@@ -15127,7 +15152,7 @@
       <c r="I212" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J212" s="130"/>
+      <c r="J212" s="125"/>
       <c r="L212" s="81" t="s">
         <v>41</v>
       </c>
@@ -15158,7 +15183,7 @@
       <c r="I213" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J213" s="130"/>
+      <c r="J213" s="125"/>
       <c r="L213" s="81" t="s">
         <v>41</v>
       </c>
@@ -15189,7 +15214,7 @@
       <c r="I214" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J214" s="130"/>
+      <c r="J214" s="125"/>
       <c r="L214" s="81" t="s">
         <v>41</v>
       </c>
@@ -15219,7 +15244,7 @@
       <c r="I215" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J215" s="130"/>
+      <c r="J215" s="125"/>
       <c r="L215" s="81" t="s">
         <v>41</v>
       </c>
@@ -15249,7 +15274,7 @@
       <c r="I216" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J216" s="130"/>
+      <c r="J216" s="125"/>
       <c r="L216" s="81" t="s">
         <v>41</v>
       </c>
@@ -15279,7 +15304,7 @@
       <c r="I217" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J217" s="130"/>
+      <c r="J217" s="125"/>
       <c r="L217" s="81" t="s">
         <v>41</v>
       </c>
@@ -15309,7 +15334,7 @@
       <c r="I218" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J218" s="130"/>
+      <c r="J218" s="125"/>
       <c r="L218" s="81" t="s">
         <v>41</v>
       </c>
@@ -15339,7 +15364,7 @@
       <c r="I219" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J219" s="130"/>
+      <c r="J219" s="125"/>
       <c r="L219" s="81" t="s">
         <v>41</v>
       </c>
@@ -15369,7 +15394,7 @@
       <c r="I220" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J220" s="130"/>
+      <c r="J220" s="125"/>
       <c r="L220" s="81" t="s">
         <v>41</v>
       </c>
@@ -15399,7 +15424,7 @@
       <c r="I221" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J221" s="130"/>
+      <c r="J221" s="125"/>
       <c r="L221" s="81" t="s">
         <v>41</v>
       </c>
@@ -15429,7 +15454,7 @@
       <c r="I222" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J222" s="130"/>
+      <c r="J222" s="125"/>
       <c r="L222" s="81" t="s">
         <v>41</v>
       </c>
@@ -15479,7 +15504,7 @@
       <c r="I224" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J224" s="131" t="s">
+      <c r="J224" s="124" t="s">
         <v>36</v>
       </c>
       <c r="L224" s="81"/>
@@ -15518,7 +15543,7 @@
       <c r="I225" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J225" s="130"/>
+      <c r="J225" s="125"/>
       <c r="L225" s="81"/>
       <c r="M225" s="94" t="s">
         <v>37</v>
@@ -15555,7 +15580,7 @@
       <c r="I226" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J226" s="130"/>
+      <c r="J226" s="125"/>
       <c r="L226" s="81"/>
       <c r="M226" s="94" t="s">
         <v>37</v>
@@ -15592,7 +15617,7 @@
       <c r="I227" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J227" s="130"/>
+      <c r="J227" s="125"/>
       <c r="L227" s="81"/>
       <c r="M227" s="94" t="s">
         <v>37</v>
@@ -15629,7 +15654,7 @@
       <c r="I228" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J228" s="130"/>
+      <c r="J228" s="125"/>
       <c r="L228" s="81"/>
       <c r="M228" s="94" t="s">
         <v>37</v>
@@ -15666,7 +15691,7 @@
       <c r="I229" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J229" s="130"/>
+      <c r="J229" s="125"/>
       <c r="L229" s="81"/>
       <c r="M229" s="94" t="s">
         <v>37</v>
@@ -15703,7 +15728,7 @@
       <c r="I230" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J230" s="130"/>
+      <c r="J230" s="125"/>
       <c r="L230" s="81"/>
       <c r="M230" s="94" t="s">
         <v>37</v>
@@ -15740,7 +15765,7 @@
       <c r="I231" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J231" s="130"/>
+      <c r="J231" s="125"/>
       <c r="L231" s="81"/>
       <c r="M231" s="94" t="s">
         <v>37</v>
@@ -15777,7 +15802,7 @@
       <c r="I232" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J232" s="130"/>
+      <c r="J232" s="125"/>
       <c r="L232" s="81"/>
       <c r="M232" s="94" t="s">
         <v>37</v>
@@ -15814,7 +15839,7 @@
       <c r="I233" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J233" s="130"/>
+      <c r="J233" s="125"/>
       <c r="L233" s="81"/>
       <c r="M233" s="94" t="s">
         <v>37</v>
@@ -15851,7 +15876,7 @@
       <c r="I234" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J234" s="130"/>
+      <c r="J234" s="125"/>
       <c r="L234" s="81"/>
       <c r="M234" s="94" t="s">
         <v>37</v>
@@ -15888,7 +15913,7 @@
       <c r="I235" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J235" s="130"/>
+      <c r="J235" s="125"/>
       <c r="L235" s="81"/>
       <c r="M235" s="94" t="s">
         <v>37</v>
@@ -15925,7 +15950,7 @@
       <c r="I236" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J236" s="130"/>
+      <c r="J236" s="125"/>
       <c r="L236" s="81"/>
       <c r="M236" s="94" t="s">
         <v>37</v>
@@ -15962,7 +15987,7 @@
       <c r="I237" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J237" s="130"/>
+      <c r="J237" s="125"/>
       <c r="L237" s="81"/>
       <c r="M237" s="94" t="s">
         <v>37</v>
@@ -15999,7 +16024,7 @@
       <c r="I238" t="s">
         <v>35</v>
       </c>
-      <c r="J238" s="130"/>
+      <c r="J238" s="125"/>
       <c r="L238" s="81"/>
       <c r="M238" s="94" t="s">
         <v>37</v>
@@ -16036,7 +16061,7 @@
       <c r="I239" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J239" s="130"/>
+      <c r="J239" s="125"/>
       <c r="L239" s="81"/>
       <c r="M239" s="94" t="s">
         <v>37</v>
@@ -16073,7 +16098,7 @@
       <c r="I240" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J240" s="130"/>
+      <c r="J240" s="125"/>
       <c r="L240" s="81"/>
       <c r="M240" s="94" t="s">
         <v>37</v>
@@ -16110,7 +16135,7 @@
       <c r="I241" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J241" s="130"/>
+      <c r="J241" s="125"/>
       <c r="L241" s="81"/>
       <c r="M241" s="94" t="s">
         <v>37</v>
@@ -16147,7 +16172,7 @@
       <c r="I242" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J242" s="130"/>
+      <c r="J242" s="125"/>
       <c r="L242" s="81"/>
       <c r="M242" s="94" t="s">
         <v>37</v>
@@ -16184,7 +16209,7 @@
       <c r="I243" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J243" s="130"/>
+      <c r="J243" s="125"/>
       <c r="L243" s="81"/>
       <c r="M243" s="94" t="s">
         <v>37</v>
@@ -16221,7 +16246,7 @@
       <c r="I244" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J244" s="130"/>
+      <c r="J244" s="125"/>
       <c r="L244" s="81"/>
       <c r="M244" s="94" t="s">
         <v>37</v>
@@ -16258,7 +16283,7 @@
       <c r="I245" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J245" s="130"/>
+      <c r="J245" s="125"/>
       <c r="L245" s="81"/>
       <c r="M245" s="94" t="s">
         <v>37</v>
@@ -16295,7 +16320,7 @@
       <c r="I246" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J246" s="130"/>
+      <c r="J246" s="125"/>
       <c r="L246" s="81"/>
       <c r="M246" s="94" t="s">
         <v>37</v>
@@ -16332,7 +16357,7 @@
       <c r="I247" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J247" s="130"/>
+      <c r="J247" s="125"/>
       <c r="L247" s="81"/>
       <c r="M247" s="94" t="s">
         <v>37</v>
@@ -16369,7 +16394,7 @@
       <c r="I248" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J248" s="130"/>
+      <c r="J248" s="125"/>
       <c r="L248" s="81"/>
       <c r="M248" s="94" t="s">
         <v>37</v>
@@ -16406,7 +16431,7 @@
       <c r="I249" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J249" s="130"/>
+      <c r="J249" s="125"/>
       <c r="L249" s="81"/>
       <c r="M249" s="94" t="s">
         <v>37</v>
@@ -16443,7 +16468,7 @@
       <c r="I250" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J250" s="130"/>
+      <c r="J250" s="125"/>
       <c r="L250" s="81"/>
       <c r="M250" s="94" t="s">
         <v>37</v>
@@ -16480,7 +16505,7 @@
       <c r="I251" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J251" s="130"/>
+      <c r="J251" s="125"/>
       <c r="L251" s="81"/>
       <c r="M251" s="94" t="s">
         <v>37</v>
@@ -16517,7 +16542,7 @@
       <c r="I252" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J252" s="130"/>
+      <c r="J252" s="125"/>
       <c r="L252" s="81"/>
       <c r="M252" s="94" t="s">
         <v>37</v>
@@ -16554,7 +16579,7 @@
       <c r="I253" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J253" s="130"/>
+      <c r="J253" s="125"/>
       <c r="L253" s="81"/>
       <c r="M253" s="94" t="s">
         <v>37</v>
@@ -16591,7 +16616,7 @@
       <c r="I254" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J254" s="130"/>
+      <c r="J254" s="125"/>
       <c r="L254" s="81"/>
       <c r="M254" s="94" t="s">
         <v>37</v>
@@ -16628,7 +16653,7 @@
       <c r="I255" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J255" s="130"/>
+      <c r="J255" s="125"/>
       <c r="L255" s="81"/>
       <c r="M255" s="94" t="s">
         <v>37</v>
@@ -16665,7 +16690,7 @@
       <c r="I256" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J256" s="130"/>
+      <c r="J256" s="125"/>
       <c r="L256" s="81"/>
       <c r="M256" s="94" t="s">
         <v>37</v>
@@ -16702,7 +16727,7 @@
       <c r="I257" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J257" s="130"/>
+      <c r="J257" s="125"/>
       <c r="L257" s="81"/>
       <c r="M257" s="94" t="s">
         <v>37</v>
@@ -16739,7 +16764,7 @@
       <c r="I258" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J258" s="130"/>
+      <c r="J258" s="125"/>
       <c r="L258" s="81"/>
       <c r="M258" s="94" t="s">
         <v>37</v>
@@ -16776,7 +16801,7 @@
       <c r="I259" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J259" s="130"/>
+      <c r="J259" s="125"/>
       <c r="L259" s="81"/>
       <c r="M259" s="94" t="s">
         <v>37</v>
@@ -16813,7 +16838,7 @@
       <c r="I260" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J260" s="130"/>
+      <c r="J260" s="125"/>
       <c r="L260" s="81"/>
       <c r="M260" s="94" t="s">
         <v>37</v>
@@ -16850,7 +16875,7 @@
       <c r="I261" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J261" s="130"/>
+      <c r="J261" s="125"/>
       <c r="L261" s="81"/>
       <c r="M261" s="94" t="s">
         <v>37</v>
@@ -16887,7 +16912,7 @@
       <c r="I262" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J262" s="130"/>
+      <c r="J262" s="125"/>
       <c r="L262" s="81"/>
       <c r="M262" s="94" t="s">
         <v>37</v>
@@ -16924,7 +16949,7 @@
       <c r="I263" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J263" s="130"/>
+      <c r="J263" s="125"/>
       <c r="L263" s="81"/>
       <c r="M263" s="94" t="s">
         <v>37</v>
@@ -16961,7 +16986,7 @@
       <c r="I264" t="s">
         <v>35</v>
       </c>
-      <c r="J264" s="130"/>
+      <c r="J264" s="125"/>
       <c r="L264" s="81"/>
       <c r="M264" s="94" t="s">
         <v>37</v>
@@ -16998,7 +17023,7 @@
       <c r="I265" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J265" s="130"/>
+      <c r="J265" s="125"/>
       <c r="L265" s="81"/>
       <c r="M265" s="94" t="s">
         <v>37</v>
@@ -17035,7 +17060,7 @@
       <c r="I266" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J266" s="130"/>
+      <c r="J266" s="125"/>
       <c r="L266" s="81"/>
       <c r="M266" s="94" t="s">
         <v>37</v>
@@ -17072,7 +17097,7 @@
       <c r="I267" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J267" s="130"/>
+      <c r="J267" s="125"/>
       <c r="L267" s="81"/>
       <c r="M267" s="94" t="s">
         <v>37</v>
@@ -17109,7 +17134,7 @@
       <c r="I268" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J268" s="130"/>
+      <c r="J268" s="125"/>
       <c r="L268" s="81"/>
       <c r="M268" s="94" t="s">
         <v>37</v>
@@ -17146,7 +17171,7 @@
       <c r="I269" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J269" s="130"/>
+      <c r="J269" s="125"/>
       <c r="L269" s="81"/>
       <c r="M269" s="94" t="s">
         <v>37</v>
@@ -17183,7 +17208,7 @@
       <c r="I270" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J270" s="130"/>
+      <c r="J270" s="125"/>
       <c r="L270" s="81"/>
       <c r="M270" s="94" t="s">
         <v>37</v>
@@ -17220,7 +17245,7 @@
       <c r="I271" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J271" s="130"/>
+      <c r="J271" s="125"/>
       <c r="L271" s="81"/>
       <c r="M271" s="94" t="s">
         <v>37</v>
@@ -17257,7 +17282,7 @@
       <c r="I272" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J272" s="130"/>
+      <c r="J272" s="125"/>
       <c r="L272" s="81"/>
       <c r="M272" s="94" t="s">
         <v>37</v>
@@ -17294,7 +17319,7 @@
       <c r="I273" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J273" s="130"/>
+      <c r="J273" s="125"/>
       <c r="L273" s="81"/>
       <c r="M273" s="94" t="s">
         <v>37</v>
@@ -17331,7 +17356,7 @@
       <c r="I274" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J274" s="130"/>
+      <c r="J274" s="125"/>
       <c r="L274" s="81"/>
       <c r="M274" s="94" t="s">
         <v>37</v>
@@ -17368,7 +17393,7 @@
       <c r="I275" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J275" s="130"/>
+      <c r="J275" s="125"/>
       <c r="L275" s="81"/>
       <c r="M275" s="94" t="s">
         <v>37</v>
@@ -17405,7 +17430,7 @@
       <c r="I276" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J276" s="130"/>
+      <c r="J276" s="125"/>
       <c r="L276" s="81"/>
       <c r="M276" s="94" t="s">
         <v>37</v>
@@ -17442,7 +17467,7 @@
       <c r="I277" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J277" s="130"/>
+      <c r="J277" s="125"/>
       <c r="L277" s="81"/>
       <c r="M277" s="94" t="s">
         <v>37</v>
@@ -17479,7 +17504,7 @@
       <c r="I278" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J278" s="130"/>
+      <c r="J278" s="125"/>
       <c r="L278" s="81"/>
       <c r="M278" s="94" t="s">
         <v>37</v>
@@ -17516,7 +17541,7 @@
       <c r="I279" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J279" s="130"/>
+      <c r="J279" s="125"/>
       <c r="L279" s="81"/>
       <c r="M279" s="94" t="s">
         <v>37</v>
@@ -17553,7 +17578,7 @@
       <c r="I280" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J280" s="130"/>
+      <c r="J280" s="125"/>
       <c r="L280" s="81"/>
       <c r="M280" s="94" t="s">
         <v>37</v>
@@ -17590,7 +17615,7 @@
       <c r="I281" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J281" s="130"/>
+      <c r="J281" s="125"/>
       <c r="L281" s="81"/>
       <c r="M281" s="94" t="s">
         <v>37</v>
@@ -17627,7 +17652,7 @@
       <c r="I282" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J282" s="130"/>
+      <c r="J282" s="125"/>
       <c r="L282" s="81"/>
       <c r="M282" s="94" t="s">
         <v>37</v>
@@ -17664,7 +17689,7 @@
       <c r="I283" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J283" s="130"/>
+      <c r="J283" s="125"/>
       <c r="L283" s="81"/>
       <c r="M283" s="94" t="s">
         <v>37</v>
@@ -17701,7 +17726,7 @@
       <c r="I284" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J284" s="130"/>
+      <c r="J284" s="125"/>
       <c r="L284" s="81"/>
       <c r="M284" s="94" t="s">
         <v>37</v>
@@ -17738,7 +17763,7 @@
       <c r="I285" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J285" s="130"/>
+      <c r="J285" s="125"/>
       <c r="L285" s="81"/>
       <c r="M285" s="94" t="s">
         <v>37</v>
@@ -17775,7 +17800,7 @@
       <c r="I286" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J286" s="130"/>
+      <c r="J286" s="125"/>
       <c r="L286" s="81"/>
       <c r="M286" s="94" t="s">
         <v>37</v>
@@ -17812,7 +17837,7 @@
       <c r="I287" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J287" s="130"/>
+      <c r="J287" s="125"/>
       <c r="L287" s="81"/>
       <c r="M287" s="94" t="s">
         <v>37</v>
@@ -17849,7 +17874,7 @@
       <c r="I288" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J288" s="130"/>
+      <c r="J288" s="125"/>
       <c r="L288" s="81"/>
       <c r="M288" s="94" t="s">
         <v>37</v>
@@ -17886,7 +17911,7 @@
       <c r="I289" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J289" s="130"/>
+      <c r="J289" s="125"/>
       <c r="L289" s="81"/>
       <c r="M289" s="94" t="s">
         <v>37</v>
@@ -17923,7 +17948,7 @@
       <c r="I290" t="s">
         <v>35</v>
       </c>
-      <c r="J290" s="130"/>
+      <c r="J290" s="125"/>
       <c r="L290" s="81"/>
       <c r="M290" s="94" t="s">
         <v>37</v>
@@ -17960,7 +17985,7 @@
       <c r="I291" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J291" s="130"/>
+      <c r="J291" s="125"/>
       <c r="L291" s="81"/>
       <c r="M291" s="94" t="s">
         <v>37</v>
@@ -17997,7 +18022,7 @@
       <c r="I292" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J292" s="130"/>
+      <c r="J292" s="125"/>
       <c r="L292" s="81"/>
       <c r="M292" s="94" t="s">
         <v>37</v>
@@ -18034,7 +18059,7 @@
       <c r="I293" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J293" s="130"/>
+      <c r="J293" s="125"/>
       <c r="L293" s="81"/>
       <c r="M293" s="94" t="s">
         <v>37</v>
@@ -18071,7 +18096,7 @@
       <c r="I294" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J294" s="130"/>
+      <c r="J294" s="125"/>
       <c r="L294" s="81"/>
       <c r="M294" s="94" t="s">
         <v>37</v>
@@ -18108,7 +18133,7 @@
       <c r="I295" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J295" s="130"/>
+      <c r="J295" s="125"/>
       <c r="L295" s="81"/>
       <c r="M295" s="94" t="s">
         <v>37</v>
@@ -18145,7 +18170,7 @@
       <c r="I296" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J296" s="130"/>
+      <c r="J296" s="125"/>
       <c r="L296" s="81"/>
       <c r="M296" s="94" t="s">
         <v>37</v>
@@ -18182,7 +18207,7 @@
       <c r="I297" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J297" s="130"/>
+      <c r="J297" s="125"/>
       <c r="L297" s="81"/>
       <c r="M297" s="94" t="s">
         <v>37</v>
@@ -18219,7 +18244,7 @@
       <c r="I298" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J298" s="130"/>
+      <c r="J298" s="125"/>
       <c r="L298" s="81"/>
       <c r="M298" s="94" t="s">
         <v>37</v>
@@ -18256,7 +18281,7 @@
       <c r="I299" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J299" s="130"/>
+      <c r="J299" s="125"/>
       <c r="L299" s="81"/>
       <c r="M299" s="94" t="s">
         <v>37</v>
@@ -18293,7 +18318,7 @@
       <c r="I300" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J300" s="130"/>
+      <c r="J300" s="125"/>
       <c r="L300" s="81"/>
       <c r="M300" s="94" t="s">
         <v>37</v>
@@ -18330,7 +18355,7 @@
       <c r="I301" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J301" s="130"/>
+      <c r="J301" s="125"/>
       <c r="L301" s="81"/>
       <c r="M301" s="94" t="s">
         <v>37</v>
@@ -18367,7 +18392,7 @@
       <c r="I302" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J302" s="130"/>
+      <c r="J302" s="125"/>
       <c r="L302" s="81"/>
       <c r="M302" s="94" t="s">
         <v>37</v>
@@ -18404,7 +18429,7 @@
       <c r="I303" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J303" s="130"/>
+      <c r="J303" s="125"/>
       <c r="L303" s="81"/>
       <c r="M303" s="94" t="s">
         <v>37</v>
@@ -18441,7 +18466,7 @@
       <c r="I304" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J304" s="130"/>
+      <c r="J304" s="125"/>
       <c r="L304" s="81"/>
       <c r="M304" s="94" t="s">
         <v>37</v>
@@ -18478,7 +18503,7 @@
       <c r="I305" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J305" s="130"/>
+      <c r="J305" s="125"/>
       <c r="L305" s="81"/>
       <c r="M305" s="94" t="s">
         <v>37</v>
@@ -18515,7 +18540,7 @@
       <c r="I306" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J306" s="130"/>
+      <c r="J306" s="125"/>
       <c r="L306" s="81"/>
       <c r="M306" s="94" t="s">
         <v>37</v>
@@ -18552,7 +18577,7 @@
       <c r="I307" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J307" s="130"/>
+      <c r="J307" s="125"/>
       <c r="L307" s="81"/>
       <c r="M307" s="94" t="s">
         <v>37</v>
@@ -18589,7 +18614,7 @@
       <c r="I308" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J308" s="130"/>
+      <c r="J308" s="125"/>
       <c r="L308" s="81"/>
       <c r="M308" s="94" t="s">
         <v>37</v>
@@ -18626,7 +18651,7 @@
       <c r="I309" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J309" s="130"/>
+      <c r="J309" s="125"/>
       <c r="L309" s="81"/>
       <c r="M309" s="94" t="s">
         <v>37</v>
@@ -18663,7 +18688,7 @@
       <c r="I310" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J310" s="130"/>
+      <c r="J310" s="125"/>
       <c r="L310" s="81"/>
       <c r="M310" s="94" t="s">
         <v>37</v>
@@ -18700,7 +18725,7 @@
       <c r="I311" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J311" s="130"/>
+      <c r="J311" s="125"/>
       <c r="L311" s="81"/>
       <c r="M311" s="94" t="s">
         <v>37</v>
@@ -18737,7 +18762,7 @@
       <c r="I312" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J312" s="130"/>
+      <c r="J312" s="125"/>
       <c r="L312" s="81"/>
       <c r="M312" s="94" t="s">
         <v>37</v>
@@ -18774,7 +18799,7 @@
       <c r="I313" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J313" s="130"/>
+      <c r="J313" s="125"/>
       <c r="L313" s="81"/>
       <c r="M313" s="94" t="s">
         <v>37</v>
@@ -18811,7 +18836,7 @@
       <c r="I314" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J314" s="130"/>
+      <c r="J314" s="125"/>
       <c r="L314" s="81"/>
       <c r="M314" s="94" t="s">
         <v>37</v>
@@ -18848,7 +18873,7 @@
       <c r="I315" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J315" s="130"/>
+      <c r="J315" s="125"/>
       <c r="L315" s="81"/>
       <c r="M315" s="94" t="s">
         <v>37</v>
@@ -18885,7 +18910,7 @@
       <c r="I316" t="s">
         <v>35</v>
       </c>
-      <c r="J316" s="130"/>
+      <c r="J316" s="125"/>
       <c r="L316" s="81"/>
       <c r="M316" s="94" t="s">
         <v>37</v>
@@ -18922,7 +18947,7 @@
       <c r="I317" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J317" s="130"/>
+      <c r="J317" s="125"/>
       <c r="L317" s="81"/>
       <c r="M317" s="94" t="s">
         <v>37</v>
@@ -18959,7 +18984,7 @@
       <c r="I318" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J318" s="130"/>
+      <c r="J318" s="125"/>
       <c r="L318" s="81"/>
       <c r="M318" s="94" t="s">
         <v>37</v>
@@ -18996,7 +19021,7 @@
       <c r="I319" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J319" s="130"/>
+      <c r="J319" s="125"/>
       <c r="L319" s="81"/>
       <c r="M319" s="94" t="s">
         <v>37</v>
@@ -19033,7 +19058,7 @@
       <c r="I320" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J320" s="130"/>
+      <c r="J320" s="125"/>
       <c r="L320" s="81"/>
       <c r="M320" s="94" t="s">
         <v>37</v>
@@ -19070,7 +19095,7 @@
       <c r="I321" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J321" s="130"/>
+      <c r="J321" s="125"/>
       <c r="L321" s="81"/>
       <c r="M321" s="94" t="s">
         <v>37</v>
@@ -19107,7 +19132,7 @@
       <c r="I322" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J322" s="130"/>
+      <c r="J322" s="125"/>
       <c r="L322" s="81"/>
       <c r="M322" s="94" t="s">
         <v>37</v>
@@ -19144,7 +19169,7 @@
       <c r="I323" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J323" s="130"/>
+      <c r="J323" s="125"/>
       <c r="L323" s="81"/>
       <c r="M323" s="94" t="s">
         <v>37</v>
@@ -19181,7 +19206,7 @@
       <c r="I324" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J324" s="130"/>
+      <c r="J324" s="125"/>
       <c r="L324" s="81"/>
       <c r="M324" s="94" t="s">
         <v>37</v>
@@ -19218,7 +19243,7 @@
       <c r="I325" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J325" s="130"/>
+      <c r="J325" s="125"/>
       <c r="L325" s="81"/>
       <c r="M325" s="94" t="s">
         <v>37</v>
@@ -19255,7 +19280,7 @@
       <c r="I326" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J326" s="130"/>
+      <c r="J326" s="125"/>
       <c r="L326" s="81"/>
       <c r="M326" s="94" t="s">
         <v>37</v>
@@ -19292,7 +19317,7 @@
       <c r="I327" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J327" s="130"/>
+      <c r="J327" s="125"/>
       <c r="L327" s="81"/>
       <c r="M327" s="94" t="s">
         <v>37</v>
@@ -19329,7 +19354,7 @@
       <c r="I328" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J328" s="130"/>
+      <c r="J328" s="125"/>
       <c r="L328" s="81"/>
       <c r="M328" s="94" t="s">
         <v>37</v>
@@ -19366,7 +19391,7 @@
       <c r="I329" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J329" s="130"/>
+      <c r="J329" s="125"/>
       <c r="L329" s="81"/>
       <c r="M329" s="94" t="s">
         <v>37</v>
@@ -19403,7 +19428,7 @@
       <c r="I330" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J330" s="130"/>
+      <c r="J330" s="125"/>
       <c r="L330" s="81"/>
       <c r="M330" s="94" t="s">
         <v>37</v>
@@ -19440,7 +19465,7 @@
       <c r="I331" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J331" s="130"/>
+      <c r="J331" s="125"/>
       <c r="L331" s="81"/>
       <c r="M331" s="94" t="s">
         <v>37</v>
@@ -19477,7 +19502,7 @@
       <c r="I332" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J332" s="130"/>
+      <c r="J332" s="125"/>
       <c r="L332" s="81"/>
       <c r="M332" s="94" t="s">
         <v>37</v>
@@ -19514,7 +19539,7 @@
       <c r="I333" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J333" s="130"/>
+      <c r="J333" s="125"/>
       <c r="L333" s="81"/>
       <c r="M333" s="94" t="s">
         <v>37</v>
@@ -19551,7 +19576,7 @@
       <c r="I334" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J334" s="130"/>
+      <c r="J334" s="125"/>
       <c r="L334" s="81"/>
       <c r="M334" s="94" t="s">
         <v>37</v>
@@ -19588,7 +19613,7 @@
       <c r="I335" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J335" s="130"/>
+      <c r="J335" s="125"/>
       <c r="L335" s="81"/>
       <c r="M335" s="94" t="s">
         <v>37</v>
@@ -19625,7 +19650,7 @@
       <c r="I336" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J336" s="130"/>
+      <c r="J336" s="125"/>
       <c r="L336" s="81"/>
       <c r="M336" s="94" t="s">
         <v>37</v>
@@ -19662,7 +19687,7 @@
       <c r="I337" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J337" s="130"/>
+      <c r="J337" s="125"/>
       <c r="L337" s="81"/>
       <c r="M337" s="94" t="s">
         <v>37</v>
@@ -19699,7 +19724,7 @@
       <c r="I338" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J338" s="130"/>
+      <c r="J338" s="125"/>
       <c r="L338" s="81"/>
       <c r="M338" s="94" t="s">
         <v>37</v>
@@ -19736,7 +19761,7 @@
       <c r="I339" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J339" s="130"/>
+      <c r="J339" s="125"/>
       <c r="L339" s="81"/>
       <c r="M339" s="94" t="s">
         <v>37</v>
@@ -19773,7 +19798,7 @@
       <c r="I340" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J340" s="130"/>
+      <c r="J340" s="125"/>
       <c r="L340" s="81"/>
       <c r="M340" s="94" t="s">
         <v>37</v>
@@ -19810,7 +19835,7 @@
       <c r="I341" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J341" s="130"/>
+      <c r="J341" s="125"/>
       <c r="L341" s="81"/>
       <c r="M341" s="94" t="s">
         <v>37</v>
@@ -19847,7 +19872,7 @@
       <c r="I342" t="s">
         <v>35</v>
       </c>
-      <c r="J342" s="130"/>
+      <c r="J342" s="125"/>
       <c r="L342" s="81"/>
       <c r="M342" s="94" t="s">
         <v>37</v>
@@ -19884,7 +19909,7 @@
       <c r="I343" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J343" s="130"/>
+      <c r="J343" s="125"/>
       <c r="L343" s="81"/>
       <c r="M343" s="94" t="s">
         <v>37</v>
@@ -19921,7 +19946,7 @@
       <c r="I344" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J344" s="130"/>
+      <c r="J344" s="125"/>
       <c r="L344" s="81"/>
       <c r="M344" s="94" t="s">
         <v>37</v>
@@ -19958,7 +19983,7 @@
       <c r="I345" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J345" s="130"/>
+      <c r="J345" s="125"/>
       <c r="L345" s="81"/>
       <c r="M345" s="94" t="s">
         <v>37</v>
@@ -19995,7 +20020,7 @@
       <c r="I346" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J346" s="130"/>
+      <c r="J346" s="125"/>
       <c r="L346" s="81"/>
       <c r="M346" s="94" t="s">
         <v>37</v>
@@ -20032,7 +20057,7 @@
       <c r="I347" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J347" s="130"/>
+      <c r="J347" s="125"/>
       <c r="L347" s="81"/>
       <c r="M347" s="94" t="s">
         <v>37</v>
@@ -20069,7 +20094,7 @@
       <c r="I348" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J348" s="130"/>
+      <c r="J348" s="125"/>
       <c r="L348" s="81"/>
       <c r="M348" s="94" t="s">
         <v>37</v>
@@ -20106,7 +20131,7 @@
       <c r="I349" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J349" s="130"/>
+      <c r="J349" s="125"/>
       <c r="L349" s="81"/>
       <c r="M349" s="94" t="s">
         <v>37</v>
@@ -20143,7 +20168,7 @@
       <c r="I350" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J350" s="130"/>
+      <c r="J350" s="125"/>
       <c r="L350" s="81"/>
       <c r="M350" s="94" t="s">
         <v>37</v>
@@ -20180,7 +20205,7 @@
       <c r="I351" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J351" s="130"/>
+      <c r="J351" s="125"/>
       <c r="L351" s="81"/>
       <c r="M351" s="94" t="s">
         <v>37</v>
@@ -20217,7 +20242,7 @@
       <c r="I352" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J352" s="130"/>
+      <c r="J352" s="125"/>
       <c r="L352" s="81"/>
       <c r="M352" s="94" t="s">
         <v>37</v>
@@ -20254,7 +20279,7 @@
       <c r="I353" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J353" s="130"/>
+      <c r="J353" s="125"/>
       <c r="L353" s="81"/>
       <c r="M353" s="94" t="s">
         <v>37</v>
@@ -20291,7 +20316,7 @@
       <c r="I354" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J354" s="130"/>
+      <c r="J354" s="125"/>
       <c r="L354" s="81"/>
       <c r="M354" s="94" t="s">
         <v>37</v>
@@ -20328,7 +20353,7 @@
       <c r="I355" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J355" s="130"/>
+      <c r="J355" s="125"/>
       <c r="L355" s="81"/>
       <c r="M355" s="94" t="s">
         <v>37</v>
@@ -20365,7 +20390,7 @@
       <c r="I356" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J356" s="130"/>
+      <c r="J356" s="125"/>
       <c r="L356" s="81"/>
       <c r="M356" s="94" t="s">
         <v>37</v>
@@ -20402,7 +20427,7 @@
       <c r="I357" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J357" s="130"/>
+      <c r="J357" s="125"/>
       <c r="L357" s="81"/>
       <c r="M357" s="94" t="s">
         <v>37</v>
@@ -20439,7 +20464,7 @@
       <c r="I358" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J358" s="130"/>
+      <c r="J358" s="125"/>
       <c r="L358" s="81"/>
       <c r="M358" s="94" t="s">
         <v>37</v>
@@ -20476,7 +20501,7 @@
       <c r="I359" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J359" s="130"/>
+      <c r="J359" s="125"/>
       <c r="L359" s="81"/>
       <c r="M359" s="94" t="s">
         <v>37</v>
@@ -20513,7 +20538,7 @@
       <c r="I360" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J360" s="130"/>
+      <c r="J360" s="125"/>
       <c r="L360" s="81"/>
       <c r="M360" s="94" t="s">
         <v>37</v>
@@ -20550,7 +20575,7 @@
       <c r="I361" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J361" s="130"/>
+      <c r="J361" s="125"/>
       <c r="L361" s="81"/>
       <c r="M361" s="94" t="s">
         <v>37</v>
@@ -20587,7 +20612,7 @@
       <c r="I362" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J362" s="130"/>
+      <c r="J362" s="125"/>
       <c r="L362" s="81"/>
       <c r="M362" s="94" t="s">
         <v>37</v>
@@ -20624,7 +20649,7 @@
       <c r="I363" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J363" s="130"/>
+      <c r="J363" s="125"/>
       <c r="L363" s="81"/>
       <c r="M363" s="94" t="s">
         <v>37</v>
@@ -20661,7 +20686,7 @@
       <c r="I364" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J364" s="130"/>
+      <c r="J364" s="125"/>
       <c r="L364" s="81"/>
       <c r="M364" s="94" t="s">
         <v>37</v>
@@ -20698,7 +20723,7 @@
       <c r="I365" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J365" s="130"/>
+      <c r="J365" s="125"/>
       <c r="L365" s="81"/>
       <c r="M365" s="94" t="s">
         <v>37</v>
@@ -20735,7 +20760,7 @@
       <c r="I366" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J366" s="130"/>
+      <c r="J366" s="125"/>
       <c r="L366" s="81"/>
       <c r="M366" s="94" t="s">
         <v>37</v>
@@ -20772,7 +20797,7 @@
       <c r="I367" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J367" s="130"/>
+      <c r="J367" s="125"/>
       <c r="L367" s="81"/>
       <c r="M367" s="94" t="s">
         <v>37</v>
@@ -20809,7 +20834,7 @@
       <c r="I368" t="s">
         <v>35</v>
       </c>
-      <c r="J368" s="130"/>
+      <c r="J368" s="125"/>
       <c r="L368" s="81"/>
       <c r="M368" s="94" t="s">
         <v>37</v>
@@ -20846,7 +20871,7 @@
       <c r="I369" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J369" s="130"/>
+      <c r="J369" s="125"/>
       <c r="L369" s="81"/>
       <c r="M369" s="94" t="s">
         <v>37</v>
@@ -20883,7 +20908,7 @@
       <c r="I370" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J370" s="130"/>
+      <c r="J370" s="125"/>
       <c r="L370" s="81"/>
       <c r="M370" s="94" t="s">
         <v>37</v>
@@ -20920,7 +20945,7 @@
       <c r="I371" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J371" s="130"/>
+      <c r="J371" s="125"/>
       <c r="L371" s="81"/>
       <c r="M371" s="94" t="s">
         <v>37</v>
@@ -20957,7 +20982,7 @@
       <c r="I372" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J372" s="130"/>
+      <c r="J372" s="125"/>
       <c r="L372" s="81"/>
       <c r="M372" s="94" t="s">
         <v>37</v>
@@ -20994,7 +21019,7 @@
       <c r="I373" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J373" s="130"/>
+      <c r="J373" s="125"/>
       <c r="L373" s="81"/>
       <c r="M373" s="94" t="s">
         <v>37</v>
@@ -21111,11 +21136,11 @@
       <c r="E378" t="s">
         <v>1435</v>
       </c>
-      <c r="F378" s="145" t="s">
+      <c r="F378" s="141" t="s">
         <v>1442</v>
       </c>
-      <c r="G378" s="146"/>
-      <c r="H378" s="146"/>
+      <c r="G378" s="142"/>
+      <c r="H378" s="142"/>
       <c r="I378" s="69" t="s">
         <v>35</v>
       </c>
@@ -21242,11 +21267,11 @@
       <c r="E383" t="s">
         <v>1435</v>
       </c>
-      <c r="F383" s="145" t="s">
+      <c r="F383" s="141" t="s">
         <v>1442</v>
       </c>
-      <c r="G383" s="146"/>
-      <c r="H383" s="146"/>
+      <c r="G383" s="142"/>
+      <c r="H383" s="142"/>
       <c r="I383" t="s">
         <v>1447</v>
       </c>
@@ -21301,7 +21326,7 @@
       <c r="I385" s="69" t="s">
         <v>515</v>
       </c>
-      <c r="J385" s="130"/>
+      <c r="J385" s="125"/>
       <c r="L385" s="81" t="s">
         <v>41</v>
       </c>
@@ -21328,7 +21353,7 @@
       <c r="I386" s="69" t="s">
         <v>515</v>
       </c>
-      <c r="J386" s="130"/>
+      <c r="J386" s="125"/>
       <c r="L386" s="81" t="s">
         <v>41</v>
       </c>
@@ -21337,33 +21362,33 @@
       </c>
     </row>
     <row r="387" spans="1:28" s="63" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A387" s="122" t="s">
+      <c r="A387" s="131" t="s">
         <v>518</v>
       </c>
-      <c r="B387" s="122"/>
-      <c r="C387" s="123"/>
-      <c r="D387" s="123"/>
-      <c r="E387" s="123"/>
-      <c r="F387" s="123"/>
-      <c r="G387" s="123"/>
-      <c r="H387" s="123"/>
-      <c r="I387" s="123"/>
-      <c r="J387" s="123"/>
-      <c r="K387" s="123"/>
-      <c r="L387" s="123"/>
-      <c r="M387" s="123"/>
-      <c r="N387" s="123"/>
-      <c r="O387" s="123"/>
-      <c r="P387" s="123"/>
-      <c r="Q387" s="123"/>
-      <c r="R387" s="123"/>
-      <c r="S387" s="123"/>
-      <c r="T387" s="123"/>
-      <c r="U387" s="123"/>
-      <c r="V387" s="123"/>
-      <c r="W387" s="123"/>
-      <c r="X387" s="123"/>
-      <c r="Y387" s="123"/>
+      <c r="B387" s="131"/>
+      <c r="C387" s="130"/>
+      <c r="D387" s="130"/>
+      <c r="E387" s="130"/>
+      <c r="F387" s="130"/>
+      <c r="G387" s="130"/>
+      <c r="H387" s="130"/>
+      <c r="I387" s="130"/>
+      <c r="J387" s="130"/>
+      <c r="K387" s="130"/>
+      <c r="L387" s="130"/>
+      <c r="M387" s="130"/>
+      <c r="N387" s="130"/>
+      <c r="O387" s="130"/>
+      <c r="P387" s="130"/>
+      <c r="Q387" s="130"/>
+      <c r="R387" s="130"/>
+      <c r="S387" s="130"/>
+      <c r="T387" s="130"/>
+      <c r="U387" s="130"/>
+      <c r="V387" s="130"/>
+      <c r="W387" s="130"/>
+      <c r="X387" s="130"/>
+      <c r="Y387" s="130"/>
       <c r="Z387" s="103"/>
       <c r="AA387" s="103"/>
       <c r="AB387" s="103"/>
@@ -21375,16 +21400,16 @@
       <c r="C388" s="59" t="s">
         <v>1429</v>
       </c>
-      <c r="E388" s="127" t="s">
+      <c r="E388" s="122" t="s">
         <v>520</v>
       </c>
-      <c r="F388" s="128"/>
-      <c r="G388" s="128"/>
-      <c r="H388" s="128"/>
+      <c r="F388" s="123"/>
+      <c r="G388" s="123"/>
+      <c r="H388" s="123"/>
       <c r="I388" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J388" s="131" t="s">
+      <c r="J388" s="124" t="s">
         <v>78</v>
       </c>
       <c r="L388" s="81" t="s">
@@ -21401,16 +21426,16 @@
       <c r="A389" t="s">
         <v>521</v>
       </c>
-      <c r="E389" s="127" t="s">
+      <c r="E389" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F389" s="128"/>
-      <c r="G389" s="128"/>
-      <c r="H389" s="128"/>
+      <c r="F389" s="123"/>
+      <c r="G389" s="123"/>
+      <c r="H389" s="123"/>
       <c r="I389" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J389" s="130"/>
+      <c r="J389" s="125"/>
       <c r="L389" s="81" t="s">
         <v>41</v>
       </c>
@@ -21425,16 +21450,16 @@
       <c r="A390" t="s">
         <v>523</v>
       </c>
-      <c r="E390" s="127" t="s">
+      <c r="E390" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F390" s="128"/>
-      <c r="G390" s="128"/>
-      <c r="H390" s="128"/>
+      <c r="F390" s="123"/>
+      <c r="G390" s="123"/>
+      <c r="H390" s="123"/>
       <c r="I390" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J390" s="130"/>
+      <c r="J390" s="125"/>
       <c r="L390" s="81" t="s">
         <v>41</v>
       </c>
@@ -21449,16 +21474,16 @@
       <c r="A391" t="s">
         <v>524</v>
       </c>
-      <c r="E391" s="127" t="s">
+      <c r="E391" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F391" s="128"/>
-      <c r="G391" s="128"/>
-      <c r="H391" s="128"/>
+      <c r="F391" s="123"/>
+      <c r="G391" s="123"/>
+      <c r="H391" s="123"/>
       <c r="I391" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J391" s="130"/>
+      <c r="J391" s="125"/>
       <c r="L391" s="81" t="s">
         <v>41</v>
       </c>
@@ -21473,16 +21498,16 @@
       <c r="A392" t="s">
         <v>525</v>
       </c>
-      <c r="E392" s="127" t="s">
+      <c r="E392" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F392" s="128"/>
-      <c r="G392" s="128"/>
-      <c r="H392" s="128"/>
+      <c r="F392" s="123"/>
+      <c r="G392" s="123"/>
+      <c r="H392" s="123"/>
       <c r="I392" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J392" s="130"/>
+      <c r="J392" s="125"/>
       <c r="L392" s="81" t="s">
         <v>41</v>
       </c>
@@ -21497,16 +21522,16 @@
       <c r="A393" t="s">
         <v>526</v>
       </c>
-      <c r="E393" s="127" t="s">
+      <c r="E393" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F393" s="128"/>
-      <c r="G393" s="128"/>
-      <c r="H393" s="128"/>
+      <c r="F393" s="123"/>
+      <c r="G393" s="123"/>
+      <c r="H393" s="123"/>
       <c r="I393" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J393" s="130"/>
+      <c r="J393" s="125"/>
       <c r="L393" s="81" t="s">
         <v>41</v>
       </c>
@@ -21521,16 +21546,16 @@
       <c r="A394" t="s">
         <v>527</v>
       </c>
-      <c r="E394" s="127" t="s">
+      <c r="E394" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F394" s="128"/>
-      <c r="G394" s="128"/>
-      <c r="H394" s="128"/>
+      <c r="F394" s="123"/>
+      <c r="G394" s="123"/>
+      <c r="H394" s="123"/>
       <c r="I394" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J394" s="130"/>
+      <c r="J394" s="125"/>
       <c r="L394" s="81" t="s">
         <v>41</v>
       </c>
@@ -21545,16 +21570,16 @@
       <c r="A395" t="s">
         <v>528</v>
       </c>
-      <c r="E395" s="127" t="s">
+      <c r="E395" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F395" s="128"/>
-      <c r="G395" s="128"/>
-      <c r="H395" s="128"/>
+      <c r="F395" s="123"/>
+      <c r="G395" s="123"/>
+      <c r="H395" s="123"/>
       <c r="I395" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J395" s="130"/>
+      <c r="J395" s="125"/>
       <c r="L395" s="81" t="s">
         <v>41</v>
       </c>
@@ -21569,16 +21594,16 @@
       <c r="A396" t="s">
         <v>529</v>
       </c>
-      <c r="E396" s="127" t="s">
+      <c r="E396" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F396" s="128"/>
-      <c r="G396" s="128"/>
-      <c r="H396" s="128"/>
+      <c r="F396" s="123"/>
+      <c r="G396" s="123"/>
+      <c r="H396" s="123"/>
       <c r="I396" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J396" s="130"/>
+      <c r="J396" s="125"/>
       <c r="L396" s="81" t="s">
         <v>41</v>
       </c>
@@ -21593,16 +21618,16 @@
       <c r="A397" t="s">
         <v>530</v>
       </c>
-      <c r="E397" s="125" t="s">
+      <c r="E397" s="126" t="s">
         <v>522</v>
       </c>
-      <c r="F397" s="126"/>
-      <c r="G397" s="126"/>
-      <c r="H397" s="126"/>
+      <c r="F397" s="127"/>
+      <c r="G397" s="127"/>
+      <c r="H397" s="127"/>
       <c r="I397" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J397" s="130"/>
+      <c r="J397" s="125"/>
       <c r="L397" s="81" t="s">
         <v>41</v>
       </c>
@@ -21614,33 +21639,33 @@
       </c>
     </row>
     <row r="398" spans="1:28" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="122" t="s">
+      <c r="A398" s="131" t="s">
         <v>531</v>
       </c>
-      <c r="B398" s="122"/>
-      <c r="C398" s="123"/>
-      <c r="D398" s="123"/>
-      <c r="E398" s="123"/>
-      <c r="F398" s="123"/>
-      <c r="G398" s="123"/>
-      <c r="H398" s="123"/>
-      <c r="I398" s="123"/>
-      <c r="J398" s="123"/>
-      <c r="K398" s="123"/>
-      <c r="L398" s="123"/>
-      <c r="M398" s="123"/>
-      <c r="N398" s="123"/>
-      <c r="O398" s="123"/>
-      <c r="P398" s="123"/>
-      <c r="Q398" s="123"/>
-      <c r="R398" s="123"/>
-      <c r="S398" s="123"/>
-      <c r="T398" s="123"/>
-      <c r="U398" s="123"/>
-      <c r="V398" s="123"/>
-      <c r="W398" s="123"/>
-      <c r="X398" s="123"/>
-      <c r="Y398" s="123"/>
+      <c r="B398" s="131"/>
+      <c r="C398" s="130"/>
+      <c r="D398" s="130"/>
+      <c r="E398" s="130"/>
+      <c r="F398" s="130"/>
+      <c r="G398" s="130"/>
+      <c r="H398" s="130"/>
+      <c r="I398" s="130"/>
+      <c r="J398" s="130"/>
+      <c r="K398" s="130"/>
+      <c r="L398" s="130"/>
+      <c r="M398" s="130"/>
+      <c r="N398" s="130"/>
+      <c r="O398" s="130"/>
+      <c r="P398" s="130"/>
+      <c r="Q398" s="130"/>
+      <c r="R398" s="130"/>
+      <c r="S398" s="130"/>
+      <c r="T398" s="130"/>
+      <c r="U398" s="130"/>
+      <c r="V398" s="130"/>
+      <c r="W398" s="130"/>
+      <c r="X398" s="130"/>
+      <c r="Y398" s="130"/>
       <c r="Z398" s="103"/>
       <c r="AA398" s="103"/>
       <c r="AB398" s="103"/>
@@ -21659,7 +21684,7 @@
         <v>83</v>
       </c>
       <c r="G399" s="36" t="s">
-        <v>147</v>
+        <v>1723</v>
       </c>
       <c r="H399" s="36" t="s">
         <v>83</v>
@@ -21667,7 +21692,9 @@
       <c r="I399" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J399" s="147"/>
+      <c r="J399" s="128" t="s">
+        <v>36</v>
+      </c>
       <c r="K399" s="74"/>
       <c r="L399" s="118" t="s">
         <v>41</v>
@@ -21718,9 +21745,11 @@
       <c r="M400" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="R400" s="93" t="s">
-        <v>37</v>
-      </c>
+      <c r="O400" s="152"/>
+      <c r="P400" s="68" t="s">
+        <v>1721</v>
+      </c>
+      <c r="R400" s="93"/>
       <c r="U400" s="17" t="s">
         <v>37</v>
       </c>
@@ -21739,7 +21768,7 @@
         <v>83</v>
       </c>
       <c r="G401" s="105" t="s">
-        <v>1703</v>
+        <v>1722</v>
       </c>
       <c r="H401" s="105" t="s">
         <v>83</v>
@@ -21780,7 +21809,7 @@
       <c r="I402" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J402" s="130"/>
+      <c r="J402" s="125"/>
       <c r="L402" s="87" t="s">
         <v>41</v>
       </c>
@@ -21813,7 +21842,7 @@
       <c r="I403" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J403" s="130"/>
+      <c r="J403" s="125"/>
       <c r="L403" s="81" t="s">
         <v>41</v>
       </c>
@@ -21846,7 +21875,7 @@
       <c r="I404" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J404" s="130"/>
+      <c r="J404" s="125"/>
       <c r="L404" s="81" t="s">
         <v>41</v>
       </c>
@@ -21879,7 +21908,7 @@
       <c r="I405" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J405" s="130"/>
+      <c r="J405" s="125"/>
       <c r="L405" s="83" t="s">
         <v>41</v>
       </c>
@@ -21912,7 +21941,7 @@
       <c r="I406" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="J406" s="126"/>
+      <c r="J406" s="127"/>
       <c r="K406" s="73"/>
       <c r="L406" s="84" t="s">
         <v>41</v>
@@ -21956,7 +21985,7 @@
       <c r="I407" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J407" s="130"/>
+      <c r="J407" s="125"/>
       <c r="L407" s="81" t="s">
         <v>41</v>
       </c>
@@ -21989,7 +22018,7 @@
       <c r="I408" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J408" s="130"/>
+      <c r="J408" s="125"/>
       <c r="L408" s="81" t="s">
         <v>41</v>
       </c>
@@ -22022,7 +22051,7 @@
       <c r="I409" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J409" s="130"/>
+      <c r="J409" s="125"/>
       <c r="L409" s="81" t="s">
         <v>41</v>
       </c>
@@ -22055,7 +22084,7 @@
       <c r="I410" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J410" s="130"/>
+      <c r="J410" s="125"/>
       <c r="L410" s="83" t="s">
         <v>41</v>
       </c>
@@ -22088,7 +22117,7 @@
       <c r="I411" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J411" s="130"/>
+      <c r="J411" s="125"/>
       <c r="L411" s="85" t="s">
         <v>41</v>
       </c>
@@ -22121,7 +22150,7 @@
       <c r="I412" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J412" s="123"/>
+      <c r="J412" s="130"/>
       <c r="K412" s="74"/>
       <c r="L412" s="86" t="s">
         <v>41</v>
@@ -22165,7 +22194,7 @@
       <c r="I413" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J413" s="130"/>
+      <c r="J413" s="125"/>
       <c r="L413" s="87" t="s">
         <v>41</v>
       </c>
@@ -22198,7 +22227,7 @@
       <c r="I414" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J414" s="130"/>
+      <c r="J414" s="125"/>
       <c r="L414" s="87" t="s">
         <v>41</v>
       </c>
@@ -22231,7 +22260,7 @@
       <c r="I415" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J415" s="130"/>
+      <c r="J415" s="125"/>
       <c r="L415" s="87" t="s">
         <v>41</v>
       </c>
@@ -22264,7 +22293,7 @@
       <c r="I416" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J416" s="130"/>
+      <c r="J416" s="125"/>
       <c r="L416" s="87" t="s">
         <v>41</v>
       </c>
@@ -22297,7 +22326,7 @@
       <c r="I417" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J417" s="130"/>
+      <c r="J417" s="125"/>
       <c r="L417" s="85" t="s">
         <v>41</v>
       </c>
@@ -22330,7 +22359,7 @@
       <c r="I418" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J418" s="130"/>
+      <c r="J418" s="125"/>
       <c r="L418" s="85" t="s">
         <v>41</v>
       </c>
@@ -22363,7 +22392,7 @@
       <c r="I419" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J419" s="123"/>
+      <c r="J419" s="130"/>
       <c r="K419" s="74"/>
       <c r="L419" s="86" t="s">
         <v>41</v>
@@ -22407,7 +22436,7 @@
       <c r="I420" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J420" s="130"/>
+      <c r="J420" s="125"/>
       <c r="L420" s="87" t="s">
         <v>41</v>
       </c>
@@ -22440,7 +22469,7 @@
       <c r="I421" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J421" s="130"/>
+      <c r="J421" s="125"/>
       <c r="L421" s="87" t="s">
         <v>41</v>
       </c>
@@ -22473,7 +22502,7 @@
       <c r="I422" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J422" s="130"/>
+      <c r="J422" s="125"/>
       <c r="L422" s="87" t="s">
         <v>41</v>
       </c>
@@ -22506,7 +22535,7 @@
       <c r="I423" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J423" s="130"/>
+      <c r="J423" s="125"/>
       <c r="L423" s="87" t="s">
         <v>41</v>
       </c>
@@ -22539,7 +22568,7 @@
       <c r="I424" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J424" s="130"/>
+      <c r="J424" s="125"/>
       <c r="L424" s="85" t="s">
         <v>41</v>
       </c>
@@ -22572,7 +22601,7 @@
       <c r="I425" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J425" s="130"/>
+      <c r="J425" s="125"/>
       <c r="L425" s="85" t="s">
         <v>41</v>
       </c>
@@ -22605,7 +22634,7 @@
       <c r="I426" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J426" s="123"/>
+      <c r="J426" s="130"/>
       <c r="K426" s="74"/>
       <c r="L426" s="86" t="s">
         <v>41</v>
@@ -22649,7 +22678,7 @@
       <c r="I427" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J427" s="130"/>
+      <c r="J427" s="125"/>
       <c r="L427" s="87" t="s">
         <v>41</v>
       </c>
@@ -22682,7 +22711,7 @@
       <c r="I428" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J428" s="130"/>
+      <c r="J428" s="125"/>
       <c r="L428" s="87" t="s">
         <v>41</v>
       </c>
@@ -22715,7 +22744,7 @@
       <c r="I429" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J429" s="130"/>
+      <c r="J429" s="125"/>
       <c r="L429" s="87" t="s">
         <v>41</v>
       </c>
@@ -22748,7 +22777,7 @@
       <c r="I430" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J430" s="130"/>
+      <c r="J430" s="125"/>
       <c r="L430" s="85" t="s">
         <v>41</v>
       </c>
@@ -22781,7 +22810,7 @@
       <c r="I431" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J431" s="130"/>
+      <c r="J431" s="125"/>
       <c r="L431" s="120" t="s">
         <v>41</v>
       </c>
@@ -22814,7 +22843,7 @@
       <c r="I432" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J432" s="130"/>
+      <c r="J432" s="125"/>
       <c r="L432" s="120" t="s">
         <v>41</v>
       </c>
@@ -22847,7 +22876,7 @@
       <c r="I433" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J433" s="123"/>
+      <c r="J433" s="130"/>
       <c r="K433" s="74"/>
       <c r="L433" s="86" t="s">
         <v>41</v>
@@ -22891,7 +22920,7 @@
       <c r="I434" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J434" s="130"/>
+      <c r="J434" s="125"/>
       <c r="L434" s="87" t="s">
         <v>41</v>
       </c>
@@ -22924,7 +22953,7 @@
       <c r="I435" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J435" s="130"/>
+      <c r="J435" s="125"/>
       <c r="L435" s="81" t="s">
         <v>41</v>
       </c>
@@ -22957,7 +22986,7 @@
       <c r="I436" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J436" s="130"/>
+      <c r="J436" s="125"/>
       <c r="L436" s="81" t="s">
         <v>41</v>
       </c>
@@ -22990,7 +23019,7 @@
       <c r="I437" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J437" s="130"/>
+      <c r="J437" s="125"/>
       <c r="L437" s="81" t="s">
         <v>41</v>
       </c>
@@ -23023,7 +23052,7 @@
       <c r="I438" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="J438" s="130"/>
+      <c r="J438" s="125"/>
       <c r="K438" s="73"/>
       <c r="L438" s="84" t="s">
         <v>41</v>
@@ -23067,7 +23096,7 @@
       <c r="I439" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J439" s="130"/>
+      <c r="J439" s="125"/>
       <c r="L439" s="81" t="s">
         <v>41</v>
       </c>
@@ -23100,7 +23129,7 @@
       <c r="I440" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J440" s="126"/>
+      <c r="J440" s="127"/>
       <c r="L440" s="81" t="s">
         <v>41</v>
       </c>
@@ -23133,7 +23162,7 @@
       <c r="I441" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J441" s="130"/>
+      <c r="J441" s="125"/>
       <c r="K441" s="74"/>
       <c r="L441" s="115" t="s">
         <v>41</v>
@@ -23174,7 +23203,7 @@
       <c r="I442" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="J442" s="130"/>
+      <c r="J442" s="125"/>
       <c r="L442" s="83" t="s">
         <v>41</v>
       </c>
@@ -23204,7 +23233,7 @@
       <c r="I443" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J443" s="130"/>
+      <c r="J443" s="125"/>
       <c r="L443" s="83" t="s">
         <v>41</v>
       </c>
@@ -23234,7 +23263,7 @@
       <c r="I444" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J444" s="130"/>
+      <c r="J444" s="125"/>
       <c r="L444" s="81" t="s">
         <v>41</v>
       </c>
@@ -23264,7 +23293,7 @@
       <c r="I445" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J445" s="130"/>
+      <c r="J445" s="125"/>
       <c r="L445" s="81" t="s">
         <v>41</v>
       </c>
@@ -23295,7 +23324,7 @@
       <c r="I446" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J446" s="130"/>
+      <c r="J446" s="125"/>
       <c r="K446" s="74"/>
       <c r="L446" s="115" t="s">
         <v>41</v>
@@ -23339,7 +23368,7 @@
       <c r="I447" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J447" s="130"/>
+      <c r="J447" s="125"/>
       <c r="L447" s="87" t="s">
         <v>41</v>
       </c>
@@ -23372,7 +23401,7 @@
       <c r="I448" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J448" s="130"/>
+      <c r="J448" s="125"/>
       <c r="L448" s="87" t="s">
         <v>41</v>
       </c>
@@ -23405,7 +23434,7 @@
       <c r="I449" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J449" s="130"/>
+      <c r="J449" s="125"/>
       <c r="L449" s="87" t="s">
         <v>41</v>
       </c>
@@ -23438,7 +23467,7 @@
       <c r="I450" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J450" s="130"/>
+      <c r="J450" s="125"/>
       <c r="L450" s="87" t="s">
         <v>41</v>
       </c>
@@ -23471,7 +23500,7 @@
       <c r="I451" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J451" s="130"/>
+      <c r="J451" s="125"/>
       <c r="K451" s="74"/>
       <c r="L451" s="115" t="s">
         <v>41</v>
@@ -23512,7 +23541,7 @@
       <c r="I452" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J452" s="130"/>
+      <c r="J452" s="125"/>
       <c r="L452" s="87" t="s">
         <v>41</v>
       </c>
@@ -23542,7 +23571,7 @@
       <c r="I453" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J453" s="130"/>
+      <c r="J453" s="125"/>
       <c r="L453" s="81" t="s">
         <v>41</v>
       </c>
@@ -23572,7 +23601,7 @@
       <c r="I454" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J454" s="130"/>
+      <c r="J454" s="125"/>
       <c r="L454" s="81" t="s">
         <v>41</v>
       </c>
@@ -23602,7 +23631,7 @@
       <c r="I455" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J455" s="130"/>
+      <c r="J455" s="125"/>
       <c r="L455" s="81" t="s">
         <v>41</v>
       </c>
@@ -23622,7 +23651,7 @@
       <c r="F456" s="38"/>
       <c r="G456" s="38"/>
       <c r="H456" s="38"/>
-      <c r="J456" s="123"/>
+      <c r="J456" s="130"/>
       <c r="K456" s="75"/>
       <c r="L456" s="88"/>
       <c r="M456" s="24"/>
@@ -23670,16 +23699,16 @@
       <c r="A459" t="s">
         <v>519</v>
       </c>
-      <c r="E459" s="127" t="s">
+      <c r="E459" s="122" t="s">
         <v>520</v>
       </c>
-      <c r="F459" s="128"/>
-      <c r="G459" s="128"/>
-      <c r="H459" s="128"/>
+      <c r="F459" s="123"/>
+      <c r="G459" s="123"/>
+      <c r="H459" s="123"/>
       <c r="I459" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J459" s="131" t="s">
+      <c r="J459" s="124" t="s">
         <v>78</v>
       </c>
       <c r="L459" s="81" t="s">
@@ -23696,16 +23725,16 @@
       <c r="A460" t="s">
         <v>521</v>
       </c>
-      <c r="E460" s="127" t="s">
+      <c r="E460" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F460" s="128"/>
-      <c r="G460" s="128"/>
-      <c r="H460" s="128"/>
+      <c r="F460" s="123"/>
+      <c r="G460" s="123"/>
+      <c r="H460" s="123"/>
       <c r="I460" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J460" s="130"/>
+      <c r="J460" s="125"/>
       <c r="L460" s="81" t="s">
         <v>41</v>
       </c>
@@ -23720,16 +23749,16 @@
       <c r="A461" t="s">
         <v>523</v>
       </c>
-      <c r="E461" s="127" t="s">
+      <c r="E461" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F461" s="128"/>
-      <c r="G461" s="128"/>
-      <c r="H461" s="128"/>
+      <c r="F461" s="123"/>
+      <c r="G461" s="123"/>
+      <c r="H461" s="123"/>
       <c r="I461" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J461" s="130"/>
+      <c r="J461" s="125"/>
       <c r="L461" s="81" t="s">
         <v>41</v>
       </c>
@@ -23744,16 +23773,16 @@
       <c r="A462" t="s">
         <v>524</v>
       </c>
-      <c r="E462" s="127" t="s">
+      <c r="E462" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F462" s="128"/>
-      <c r="G462" s="128"/>
-      <c r="H462" s="128"/>
+      <c r="F462" s="123"/>
+      <c r="G462" s="123"/>
+      <c r="H462" s="123"/>
       <c r="I462" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J462" s="130"/>
+      <c r="J462" s="125"/>
       <c r="L462" s="81" t="s">
         <v>41</v>
       </c>
@@ -23768,16 +23797,16 @@
       <c r="A463" t="s">
         <v>525</v>
       </c>
-      <c r="E463" s="127" t="s">
+      <c r="E463" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F463" s="128"/>
-      <c r="G463" s="128"/>
-      <c r="H463" s="128"/>
+      <c r="F463" s="123"/>
+      <c r="G463" s="123"/>
+      <c r="H463" s="123"/>
       <c r="I463" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J463" s="130"/>
+      <c r="J463" s="125"/>
       <c r="L463" s="81" t="s">
         <v>41</v>
       </c>
@@ -23792,16 +23821,16 @@
       <c r="A464" t="s">
         <v>526</v>
       </c>
-      <c r="E464" s="127" t="s">
+      <c r="E464" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F464" s="128"/>
-      <c r="G464" s="128"/>
-      <c r="H464" s="128"/>
+      <c r="F464" s="123"/>
+      <c r="G464" s="123"/>
+      <c r="H464" s="123"/>
       <c r="I464" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J464" s="130"/>
+      <c r="J464" s="125"/>
       <c r="L464" s="81" t="s">
         <v>41</v>
       </c>
@@ -23816,16 +23845,16 @@
       <c r="A465" t="s">
         <v>527</v>
       </c>
-      <c r="E465" s="127" t="s">
+      <c r="E465" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F465" s="128"/>
-      <c r="G465" s="128"/>
-      <c r="H465" s="128"/>
+      <c r="F465" s="123"/>
+      <c r="G465" s="123"/>
+      <c r="H465" s="123"/>
       <c r="I465" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J465" s="130"/>
+      <c r="J465" s="125"/>
       <c r="L465" s="81" t="s">
         <v>41</v>
       </c>
@@ -23840,16 +23869,16 @@
       <c r="A466" t="s">
         <v>528</v>
       </c>
-      <c r="E466" s="127" t="s">
+      <c r="E466" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F466" s="128"/>
-      <c r="G466" s="128"/>
-      <c r="H466" s="128"/>
+      <c r="F466" s="123"/>
+      <c r="G466" s="123"/>
+      <c r="H466" s="123"/>
       <c r="I466" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J466" s="130"/>
+      <c r="J466" s="125"/>
       <c r="L466" s="81" t="s">
         <v>41</v>
       </c>
@@ -23864,16 +23893,16 @@
       <c r="A467" t="s">
         <v>529</v>
       </c>
-      <c r="E467" s="127" t="s">
+      <c r="E467" s="122" t="s">
         <v>522</v>
       </c>
-      <c r="F467" s="128"/>
-      <c r="G467" s="128"/>
-      <c r="H467" s="128"/>
+      <c r="F467" s="123"/>
+      <c r="G467" s="123"/>
+      <c r="H467" s="123"/>
       <c r="I467" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J467" s="130"/>
+      <c r="J467" s="125"/>
       <c r="L467" s="81" t="s">
         <v>41</v>
       </c>
@@ -23888,16 +23917,16 @@
       <c r="A468" t="s">
         <v>530</v>
       </c>
-      <c r="E468" s="125" t="s">
+      <c r="E468" s="126" t="s">
         <v>522</v>
       </c>
-      <c r="F468" s="126"/>
-      <c r="G468" s="126"/>
-      <c r="H468" s="126"/>
+      <c r="F468" s="127"/>
+      <c r="G468" s="127"/>
+      <c r="H468" s="127"/>
       <c r="I468" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="J468" s="130"/>
+      <c r="J468" s="125"/>
       <c r="L468" s="81" t="s">
         <v>41</v>
       </c>
@@ -23910,6 +23939,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A398:Y398"/>
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="E397:H397"/>
+    <mergeCell ref="E391:H391"/>
+    <mergeCell ref="E392:H392"/>
+    <mergeCell ref="E393:H393"/>
+    <mergeCell ref="E394:H394"/>
+    <mergeCell ref="J38:J61"/>
+    <mergeCell ref="J385:J386"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="E388:H388"/>
+    <mergeCell ref="J26:J36"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="E396:H396"/>
+    <mergeCell ref="J184:J222"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="A387:Y387"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A7:Y7"/>
+    <mergeCell ref="J224:J373"/>
+    <mergeCell ref="A134:Y134"/>
+    <mergeCell ref="A25:Y25"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="F378:H378"/>
+    <mergeCell ref="F383:H383"/>
     <mergeCell ref="E390:H390"/>
     <mergeCell ref="J388:J397"/>
     <mergeCell ref="E395:H395"/>
@@ -23926,35 +23984,6 @@
     <mergeCell ref="E468:H468"/>
     <mergeCell ref="E389:H389"/>
     <mergeCell ref="J399:J456"/>
-    <mergeCell ref="A387:Y387"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A7:Y7"/>
-    <mergeCell ref="J224:J373"/>
-    <mergeCell ref="A134:Y134"/>
-    <mergeCell ref="A25:Y25"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="F378:H378"/>
-    <mergeCell ref="F383:H383"/>
-    <mergeCell ref="A398:Y398"/>
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="E397:H397"/>
-    <mergeCell ref="E391:H391"/>
-    <mergeCell ref="E392:H392"/>
-    <mergeCell ref="E393:H393"/>
-    <mergeCell ref="E394:H394"/>
-    <mergeCell ref="J38:J61"/>
-    <mergeCell ref="J385:J386"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="E388:H388"/>
-    <mergeCell ref="J26:J36"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="E396:H396"/>
-    <mergeCell ref="J184:J222"/>
-    <mergeCell ref="D1:H1"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{CF2F4C45-979B-4FC4-A73B-26D7DFB68EE4}">
@@ -24018,21 +24047,21 @@
       <c r="F1" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="G1" s="124"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
@@ -24049,20 +24078,20 @@
       <c r="H2" s="148" t="s">
         <v>545</v>
       </c>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="133"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="135"/>
       <c r="P2" s="149" t="s">
         <v>546</v>
       </c>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128"/>
-      <c r="S2" s="128"/>
-      <c r="T2" s="133"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="135"/>
     </row>
     <row r="3" spans="1:25" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="70" t="s">
@@ -24071,16 +24100,16 @@
       <c r="H3" s="19" t="s">
         <v>547</v>
       </c>
-      <c r="I3" s="139" t="s">
+      <c r="I3" s="134" t="s">
         <v>548</v>
       </c>
-      <c r="J3" s="133"/>
+      <c r="J3" s="135"/>
       <c r="K3" s="150" t="s">
         <v>549</v>
       </c>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="133"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="135"/>
       <c r="O3" s="20" t="s">
         <v>550</v>
       </c>
@@ -24093,8 +24122,8 @@
       <c r="R3" s="151" t="s">
         <v>552</v>
       </c>
-      <c r="S3" s="128"/>
-      <c r="T3" s="133"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="135"/>
     </row>
     <row r="4" spans="1:25" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="2" t="s">
@@ -31447,34 +31476,34 @@
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="136"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="147"/>
       <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="124"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="130"/>
+      <c r="X1" s="130"/>
+      <c r="Y1" s="130"/>
     </row>
     <row r="2" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="68"/>
@@ -31487,16 +31516,16 @@
       <c r="L2" s="19" t="s">
         <v>1169</v>
       </c>
-      <c r="M2" s="139" t="s">
+      <c r="M2" s="134" t="s">
         <v>1170</v>
       </c>
-      <c r="N2" s="133"/>
-      <c r="O2" s="142" t="s">
+      <c r="N2" s="135"/>
+      <c r="O2" s="138" t="s">
         <v>1171</v>
       </c>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="144"/>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="139"/>
+      <c r="R2" s="140"/>
       <c r="S2" s="29" t="s">
         <v>1172</v>
       </c>
@@ -31506,11 +31535,11 @@
       <c r="U2" s="31" t="s">
         <v>1174</v>
       </c>
-      <c r="V2" s="132" t="s">
+      <c r="V2" s="144" t="s">
         <v>1175</v>
       </c>
-      <c r="W2" s="128"/>
-      <c r="X2" s="133"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="135"/>
     </row>
     <row r="3" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>